<commit_message>
Auchann Integratie, Backplacement of replacements and noncompletions
</commit_message>
<xml_diff>
--- a/methods/STAP_Index_Current.xlsx
+++ b/methods/STAP_Index_Current.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\jodijk\Dropbox\jodijk\Utrecht\Projects\CLARIAH CORE\WP3\VKL\STAP\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox\jodijk\myprograms\python\sastacode\mysastadev\methods\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7089E4B5-AB9E-4872-A835-4885C7CF49D4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC663DBB-7600-4C3D-A5D9-C3609F9A2B79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="12360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -392,18 +392,6 @@
     <t>core</t>
   </si>
   <si>
-    <t xml:space="preserve">//node[@cat="cp"
-    or @cat="whrel"
-    or @cat="whsub"
-    or @cat= "rel" 
-    or (node[@cat="ssub"]
-        and @rel!="body" 
-        and @rel!="cnj" 
-        and @rel!="tag" 
-        and @rel!="nucl")]
-</t>
-  </si>
-  <si>
     <t>S013</t>
   </si>
   <si>
@@ -557,6 +545,18 @@
   </si>
   <si>
     <t>Forms</t>
+  </si>
+  <si>
+    <t xml:space="preserve">//node[(@cat="cp" and node[@cat="ssub"])
+    or @cat="whrel"
+    or @cat="whsub"
+    or @cat= "rel" 
+    or (node[@cat="ssub"]
+        and @rel!="body" 
+        and @rel!="cnj" 
+        and @rel!="tag" 
+        and @rel!="nucl")]
+</t>
   </si>
 </sst>
 </file>
@@ -994,10 +994,10 @@
   <dimension ref="A1:Q148"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="5" ySplit="1" topLeftCell="I17" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="1" topLeftCell="I2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="M20" sqref="M20"/>
+      <selection pane="bottomRight" activeCell="K4" sqref="K4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1095,7 +1095,7 @@
         <v>97</v>
       </c>
       <c r="K2" s="9" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="L2" s="2" t="s">
         <v>98</v>
@@ -1133,7 +1133,7 @@
         <v>97</v>
       </c>
       <c r="K3" s="9" t="s">
-        <v>108</v>
+        <v>151</v>
       </c>
       <c r="L3" s="2" t="s">
         <v>98</v>
@@ -1171,7 +1171,7 @@
         <v>97</v>
       </c>
       <c r="K4" s="9" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="L4" s="2" t="s">
         <v>98</v>
@@ -1212,7 +1212,7 @@
         <v>97</v>
       </c>
       <c r="K5" s="9" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="L5" s="2" t="s">
         <v>98</v>
@@ -1326,7 +1326,7 @@
         <v>97</v>
       </c>
       <c r="K8" s="9" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="L8" s="2" t="s">
         <v>98</v>
@@ -1367,7 +1367,7 @@
         <v>97</v>
       </c>
       <c r="K9" s="9" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="L9" s="2" t="s">
         <v>98</v>
@@ -1408,7 +1408,7 @@
         <v>97</v>
       </c>
       <c r="K10" s="9" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="L10" s="2" t="s">
         <v>98</v>
@@ -1446,7 +1446,7 @@
         <v>97</v>
       </c>
       <c r="K11" s="9" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="L11" s="2" t="s">
         <v>98</v>
@@ -1484,7 +1484,7 @@
         <v>97</v>
       </c>
       <c r="K12" s="9" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="L12" s="2" t="s">
         <v>98</v>
@@ -1522,7 +1522,7 @@
         <v>97</v>
       </c>
       <c r="K13" s="9" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="L13" s="2" t="s">
         <v>98</v>
@@ -1536,19 +1536,19 @@
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="B14" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="C14" s="2" t="s">
         <v>110</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>111</v>
       </c>
       <c r="D14" s="2" t="s">
         <v>99</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="H14" s="2" t="s">
         <v>98</v>
@@ -1560,7 +1560,7 @@
         <v>97</v>
       </c>
       <c r="K14" s="9" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="L14" s="2" t="s">
         <v>98</v>
@@ -1569,36 +1569,36 @@
         <v>98</v>
       </c>
       <c r="N14" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D15" s="2" t="s">
         <v>99</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="H15" s="2" t="s">
         <v>98</v>
       </c>
       <c r="I15" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="J15" s="2" t="s">
         <v>97</v>
       </c>
       <c r="K15" s="9" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="L15" s="2" t="s">
         <v>98</v>
@@ -1607,36 +1607,36 @@
         <v>98</v>
       </c>
       <c r="N15" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D16" s="2" t="s">
         <v>99</v>
       </c>
       <c r="E16" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="H16" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="I16" s="2" t="s">
         <v>121</v>
-      </c>
-      <c r="H16" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="I16" s="2" t="s">
-        <v>122</v>
       </c>
       <c r="J16" s="2" t="s">
         <v>97</v>
       </c>
       <c r="K16" s="9" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="L16" s="2" t="s">
         <v>98</v>
@@ -1645,30 +1645,30 @@
         <v>98</v>
       </c>
       <c r="N16" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="17" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D17" s="2" t="s">
         <v>99</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="H17" s="2" t="s">
         <v>98</v>
       </c>
       <c r="I17" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="J17" s="2" t="s">
         <v>97</v>
@@ -1680,33 +1680,33 @@
         <v>98</v>
       </c>
       <c r="N17" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="Q17" s="9" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D18" s="2" t="s">
         <v>99</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="H18" s="2" t="s">
         <v>98</v>
       </c>
       <c r="I18" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="J18" s="2" t="s">
         <v>97</v>
@@ -1718,33 +1718,33 @@
         <v>98</v>
       </c>
       <c r="N18" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="Q18" s="10" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="19" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D19" s="6" t="s">
         <v>99</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="H19" s="2" t="s">
         <v>98</v>
       </c>
       <c r="I19" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="J19" s="2" t="s">
         <v>97</v>
@@ -1756,33 +1756,33 @@
         <v>98</v>
       </c>
       <c r="N19" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="Q19" s="9" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="E20" s="2" t="s">
         <v>148</v>
       </c>
-      <c r="B20" s="2" t="s">
-        <v>151</v>
-      </c>
-      <c r="E20" s="2" t="s">
+      <c r="H20" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="K20" s="9" t="s">
         <v>149</v>
       </c>
-      <c r="H20" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="K20" s="9" t="s">
-        <v>150</v>
-      </c>
       <c r="L20" s="2" t="s">
         <v>98</v>
       </c>
       <c r="N20" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="24" spans="1:17" x14ac:dyDescent="0.3">

</xml_diff>